<commit_message>
math121: Section 2p1 written
</commit_message>
<xml_diff>
--- a/annuity_scratchwork.xlsx
+++ b/annuity_scratchwork.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Future value" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Present value" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -32,15 +33,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -100,12 +103,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -126,13 +133,103 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <f aca="false">$A$1*(1+$B$1)^($A$7-A3)</f>
+        <v>146.41</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <f aca="false">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <f aca="false">$A$1*(1+$B$1)^($A$7-A4)</f>
+        <v>133.1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <f aca="false">A4+1</f>
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <f aca="false">$A$1*(1+$B$1)^($A$7-A5)</f>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <f aca="false">A5+1</f>
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <f aca="false">$A$1*(1+$B$1)^($A$7-A6)</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
+        <f aca="false">A6+1</f>
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <f aca="false">$A$1*(1+$B$1)^($A$7-A7)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="n">
+        <f aca="false">SUM(B3:B7)</f>
+        <v>610.51</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="2" width="11.54"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">

</xml_diff>